<commit_message>
merge with VietAnh and add class crawlerDataHOSE CAFEF!
</commit_message>
<xml_diff>
--- a/test/stock.xlsx
+++ b/test/stock.xlsx
@@ -49,6 +49,33 @@
     <t>MinPrice</t>
   </si>
   <si>
+    <t>03/06/2020</t>
+  </si>
+  <si>
+    <t>881.17</t>
+  </si>
+  <si>
+    <t>6.37điểm (0.73 %)</t>
+  </si>
+  <si>
+    <t>310,662,830</t>
+  </si>
+  <si>
+    <t>4,295,391,000,000</t>
+  </si>
+  <si>
+    <t>15,834,001</t>
+  </si>
+  <si>
+    <t>366,424,002,900</t>
+  </si>
+  <si>
+    <t>876.73</t>
+  </si>
+  <si>
+    <t>874.01</t>
+  </si>
+  <si>
     <t>02/06/2020</t>
   </si>
   <si>
@@ -592,435 +619,438 @@
     <t>782.59</t>
   </si>
   <si>
+    <t>55.98</t>
+  </si>
+  <si>
+    <t>0.39điểm (0.71 %)</t>
+  </si>
+  <si>
+    <t>48,605,296</t>
+  </si>
+  <si>
+    <t>496,065,618,900</t>
+  </si>
+  <si>
+    <t>2,629,750</t>
+  </si>
+  <si>
+    <t>37,372,147,600</t>
+  </si>
+  <si>
+    <t>55.58</t>
+  </si>
+  <si>
+    <t>56.25</t>
+  </si>
+  <si>
+    <t>55.55</t>
+  </si>
+  <si>
+    <t>55.59</t>
+  </si>
+  <si>
+    <t>0.56điểm (1.01 %)</t>
+  </si>
+  <si>
+    <t>26,383,384</t>
+  </si>
+  <si>
+    <t>343,152,646,900</t>
+  </si>
+  <si>
+    <t>723,960</t>
+  </si>
+  <si>
+    <t>34,501,124,000</t>
+  </si>
+  <si>
+    <t>55.04</t>
+  </si>
+  <si>
+    <t>55.67</t>
+  </si>
+  <si>
+    <t>54.97</t>
+  </si>
+  <si>
+    <t>55.03</t>
+  </si>
+  <si>
+    <t>0.02điểm (0.03 %)</t>
+  </si>
+  <si>
+    <t>22,450,943</t>
+  </si>
+  <si>
+    <t>272,663,738,000</t>
+  </si>
+  <si>
+    <t>4,126,924</t>
+  </si>
+  <si>
+    <t>50,960,593,700</t>
+  </si>
+  <si>
+    <t>55.02</t>
+  </si>
+  <si>
+    <t>55.20</t>
+  </si>
+  <si>
+    <t>54.84</t>
+  </si>
+  <si>
+    <t>55.01</t>
+  </si>
+  <si>
+    <t>0.09điểm (0.16 %)</t>
+  </si>
+  <si>
+    <t>12,509,084</t>
+  </si>
+  <si>
+    <t>194,348,832,300</t>
+  </si>
+  <si>
+    <t>1,314,640</t>
+  </si>
+  <si>
+    <t>27,616,399,600</t>
+  </si>
+  <si>
+    <t>54.92</t>
+  </si>
+  <si>
+    <t>55.15</t>
+  </si>
+  <si>
+    <t>54.90</t>
+  </si>
+  <si>
+    <t>54.93</t>
+  </si>
+  <si>
+    <t>-0.40điểm (-0.72 %)</t>
+  </si>
+  <si>
+    <t>24,857,154</t>
+  </si>
+  <si>
+    <t>329,406,940,900</t>
+  </si>
+  <si>
+    <t>1,468,905</t>
+  </si>
+  <si>
+    <t>151,601,809,000</t>
+  </si>
+  <si>
+    <t>55.33</t>
+  </si>
+  <si>
+    <t>55.60</t>
+  </si>
+  <si>
+    <t>19,674,005</t>
+  </si>
+  <si>
+    <t>264,898,434,300</t>
+  </si>
+  <si>
+    <t>763,714</t>
+  </si>
+  <si>
+    <t>18,084,410,200</t>
+  </si>
+  <si>
+    <t>54.88</t>
+  </si>
+  <si>
+    <t>0.69điểm (1.28 %)</t>
+  </si>
+  <si>
+    <t>16,388,585</t>
+  </si>
+  <si>
+    <t>257,469,684,500</t>
+  </si>
+  <si>
+    <t>8,691,024</t>
+  </si>
+  <si>
+    <t>554,832,119,200</t>
+  </si>
+  <si>
+    <t>54.24</t>
+  </si>
+  <si>
+    <t>54.22</t>
+  </si>
+  <si>
+    <t>-0.07điểm (-0.13 %)</t>
+  </si>
+  <si>
+    <t>24,243,651</t>
+  </si>
+  <si>
+    <t>279,507,059,400</t>
+  </si>
+  <si>
+    <t>291,986</t>
+  </si>
+  <si>
+    <t>2,208,249,800</t>
+  </si>
+  <si>
+    <t>54.32</t>
+  </si>
+  <si>
+    <t>54.48</t>
+  </si>
+  <si>
+    <t>54.07</t>
+  </si>
+  <si>
+    <t>54.31</t>
+  </si>
+  <si>
+    <t>0.30điểm (0.55 %)</t>
+  </si>
+  <si>
+    <t>13,608,188</t>
+  </si>
+  <si>
+    <t>215,509,098,300</t>
+  </si>
+  <si>
+    <t>1,763,277</t>
+  </si>
+  <si>
+    <t>39,443,629,000</t>
+  </si>
+  <si>
+    <t>54.00</t>
+  </si>
+  <si>
+    <t>54.36</t>
+  </si>
+  <si>
+    <t>53.98</t>
+  </si>
+  <si>
+    <t>54.01</t>
+  </si>
+  <si>
+    <t>0.22điểm (0.40 %)</t>
+  </si>
+  <si>
+    <t>16,734,191</t>
+  </si>
+  <si>
+    <t>276,005,006,400</t>
+  </si>
+  <si>
+    <t>2,346,593</t>
+  </si>
+  <si>
+    <t>179,457,150,700</t>
+  </si>
+  <si>
+    <t>53.80</t>
+  </si>
+  <si>
+    <t>54.15</t>
+  </si>
+  <si>
+    <t>53.75</t>
+  </si>
+  <si>
+    <t>0.51điểm (0.96 %)</t>
+  </si>
+  <si>
+    <t>21,927,340</t>
+  </si>
+  <si>
+    <t>318,558,925,300</t>
+  </si>
+  <si>
+    <t>25,253,065</t>
+  </si>
+  <si>
+    <t>1,019,772,796,600</t>
+  </si>
+  <si>
+    <t>53.29</t>
+  </si>
+  <si>
+    <t>53.28</t>
+  </si>
+  <si>
+    <t>0.13điểm (0.25 %)</t>
+  </si>
+  <si>
+    <t>14,045,023</t>
+  </si>
+  <si>
+    <t>215,456,439,600</t>
+  </si>
+  <si>
+    <t>3,941,461</t>
+  </si>
+  <si>
+    <t>233,296,941,810</t>
+  </si>
+  <si>
+    <t>53.15</t>
+  </si>
+  <si>
+    <t>53.31</t>
+  </si>
+  <si>
+    <t>53.01</t>
+  </si>
+  <si>
+    <t>-0.33điểm (-0.62 %)</t>
+  </si>
+  <si>
+    <t>26,799,134</t>
+  </si>
+  <si>
+    <t>247,055,599,600</t>
+  </si>
+  <si>
+    <t>598,859</t>
+  </si>
+  <si>
+    <t>11,903,812,900</t>
+  </si>
+  <si>
+    <t>53.48</t>
+  </si>
+  <si>
+    <t>53.61</t>
+  </si>
+  <si>
+    <t>53.11</t>
+  </si>
+  <si>
+    <t>-0.24điểm (-0.45 %)</t>
+  </si>
+  <si>
+    <t>22,960,179</t>
+  </si>
+  <si>
+    <t>297,707,086,700</t>
+  </si>
+  <si>
+    <t>76,719</t>
+  </si>
+  <si>
+    <t>2,809,190,000</t>
+  </si>
+  <si>
+    <t>53.73</t>
+  </si>
+  <si>
+    <t>53.44</t>
+  </si>
+  <si>
+    <t>53.63</t>
+  </si>
+  <si>
+    <t>0.14điểm (0.27 %)</t>
+  </si>
+  <si>
+    <t>19,483,075</t>
+  </si>
+  <si>
+    <t>254,194,013,600</t>
+  </si>
+  <si>
+    <t>1,036,090</t>
+  </si>
+  <si>
+    <t>24,788,234,000</t>
+  </si>
+  <si>
+    <t>53.49</t>
+  </si>
+  <si>
+    <t>0.59điểm (1.11 %)</t>
+  </si>
+  <si>
+    <t>24,341,876</t>
+  </si>
+  <si>
+    <t>311,148,985,800</t>
+  </si>
+  <si>
+    <t>175,141</t>
+  </si>
+  <si>
+    <t>1,768,310,000</t>
+  </si>
+  <si>
+    <t>52.90</t>
+  </si>
+  <si>
+    <t>52.91</t>
+  </si>
+  <si>
+    <t>0.54điểm (1.03 %)</t>
+  </si>
+  <si>
+    <t>31,651,876</t>
+  </si>
+  <si>
+    <t>325,625,182,700</t>
+  </si>
+  <si>
+    <t>1,851,305</t>
+  </si>
+  <si>
+    <t>50,691,392,500</t>
+  </si>
+  <si>
+    <t>52.36</t>
+  </si>
+  <si>
+    <t>53.13</t>
+  </si>
+  <si>
+    <t>52.28</t>
+  </si>
+  <si>
+    <t>52.37</t>
+  </si>
+  <si>
+    <t>0.02điểm (0.04 %)</t>
+  </si>
+  <si>
+    <t>14,613,385</t>
+  </si>
+  <si>
+    <t>213,543,324,400</t>
+  </si>
+  <si>
+    <t>881,282</t>
+  </si>
+  <si>
+    <t>23,594,070,800</t>
+  </si>
+  <si>
+    <t>52.35</t>
+  </si>
+  <si>
+    <t>52.46</t>
+  </si>
+  <si>
+    <t>52.21</t>
+  </si>
+  <si>
     <t>06/05/2020</t>
   </si>
   <si>
-    <t>18.43điểm (2.41 %)</t>
-  </si>
-  <si>
-    <t>201,354,240</t>
-  </si>
-  <si>
-    <t>3,429,446,950,000</t>
-  </si>
-  <si>
-    <t>61,989,928</t>
-  </si>
-  <si>
-    <t>2,878,541,911,900</t>
-  </si>
-  <si>
-    <t>767.30</t>
-  </si>
-  <si>
-    <t>765.37</t>
-  </si>
-  <si>
-    <t>55.59</t>
-  </si>
-  <si>
-    <t>0.56điểm (1.01 %)</t>
-  </si>
-  <si>
-    <t>26,383,384</t>
-  </si>
-  <si>
-    <t>343,152,646,900</t>
-  </si>
-  <si>
-    <t>723,960</t>
-  </si>
-  <si>
-    <t>34,501,124,000</t>
-  </si>
-  <si>
-    <t>55.04</t>
-  </si>
-  <si>
-    <t>55.67</t>
-  </si>
-  <si>
-    <t>54.97</t>
-  </si>
-  <si>
-    <t>55.03</t>
-  </si>
-  <si>
-    <t>0.02điểm (0.03 %)</t>
-  </si>
-  <si>
-    <t>22,450,943</t>
-  </si>
-  <si>
-    <t>272,663,738,000</t>
-  </si>
-  <si>
-    <t>4,126,924</t>
-  </si>
-  <si>
-    <t>50,960,593,700</t>
-  </si>
-  <si>
-    <t>55.02</t>
-  </si>
-  <si>
-    <t>55.20</t>
-  </si>
-  <si>
-    <t>54.84</t>
-  </si>
-  <si>
-    <t>55.01</t>
-  </si>
-  <si>
-    <t>0.09điểm (0.16 %)</t>
-  </si>
-  <si>
-    <t>12,509,084</t>
-  </si>
-  <si>
-    <t>194,348,832,300</t>
-  </si>
-  <si>
-    <t>1,314,640</t>
-  </si>
-  <si>
-    <t>27,616,399,600</t>
-  </si>
-  <si>
-    <t>54.92</t>
-  </si>
-  <si>
-    <t>55.15</t>
-  </si>
-  <si>
-    <t>54.90</t>
-  </si>
-  <si>
-    <t>54.93</t>
-  </si>
-  <si>
-    <t>-0.40điểm (-0.72 %)</t>
-  </si>
-  <si>
-    <t>24,857,154</t>
-  </si>
-  <si>
-    <t>329,406,940,900</t>
-  </si>
-  <si>
-    <t>1,468,905</t>
-  </si>
-  <si>
-    <t>151,601,809,000</t>
-  </si>
-  <si>
-    <t>55.33</t>
-  </si>
-  <si>
-    <t>55.60</t>
-  </si>
-  <si>
-    <t>0.39điểm (0.71 %)</t>
-  </si>
-  <si>
-    <t>19,674,005</t>
-  </si>
-  <si>
-    <t>264,898,434,300</t>
-  </si>
-  <si>
-    <t>763,714</t>
-  </si>
-  <si>
-    <t>18,084,410,200</t>
-  </si>
-  <si>
-    <t>54.88</t>
-  </si>
-  <si>
-    <t>0.69điểm (1.28 %)</t>
-  </si>
-  <si>
-    <t>16,388,585</t>
-  </si>
-  <si>
-    <t>257,469,684,500</t>
-  </si>
-  <si>
-    <t>8,691,024</t>
-  </si>
-  <si>
-    <t>554,832,119,200</t>
-  </si>
-  <si>
-    <t>54.24</t>
-  </si>
-  <si>
-    <t>54.22</t>
-  </si>
-  <si>
-    <t>-0.07điểm (-0.13 %)</t>
-  </si>
-  <si>
-    <t>24,243,651</t>
-  </si>
-  <si>
-    <t>279,507,059,400</t>
-  </si>
-  <si>
-    <t>291,986</t>
-  </si>
-  <si>
-    <t>2,208,249,800</t>
-  </si>
-  <si>
-    <t>54.32</t>
-  </si>
-  <si>
-    <t>54.48</t>
-  </si>
-  <si>
-    <t>54.07</t>
-  </si>
-  <si>
-    <t>54.31</t>
-  </si>
-  <si>
-    <t>0.30điểm (0.55 %)</t>
-  </si>
-  <si>
-    <t>13,608,188</t>
-  </si>
-  <si>
-    <t>215,509,098,300</t>
-  </si>
-  <si>
-    <t>1,763,277</t>
-  </si>
-  <si>
-    <t>39,443,629,000</t>
-  </si>
-  <si>
-    <t>54.00</t>
-  </si>
-  <si>
-    <t>54.36</t>
-  </si>
-  <si>
-    <t>53.98</t>
-  </si>
-  <si>
-    <t>54.01</t>
-  </si>
-  <si>
-    <t>0.22điểm (0.40 %)</t>
-  </si>
-  <si>
-    <t>16,734,191</t>
-  </si>
-  <si>
-    <t>276,005,006,400</t>
-  </si>
-  <si>
-    <t>2,346,593</t>
-  </si>
-  <si>
-    <t>179,457,150,700</t>
-  </si>
-  <si>
-    <t>53.80</t>
-  </si>
-  <si>
-    <t>54.15</t>
-  </si>
-  <si>
-    <t>53.75</t>
-  </si>
-  <si>
-    <t>0.51điểm (0.96 %)</t>
-  </si>
-  <si>
-    <t>21,927,340</t>
-  </si>
-  <si>
-    <t>318,558,925,300</t>
-  </si>
-  <si>
-    <t>25,253,065</t>
-  </si>
-  <si>
-    <t>1,019,772,796,600</t>
-  </si>
-  <si>
-    <t>53.29</t>
-  </si>
-  <si>
-    <t>53.28</t>
-  </si>
-  <si>
-    <t>0.13điểm (0.25 %)</t>
-  </si>
-  <si>
-    <t>14,045,023</t>
-  </si>
-  <si>
-    <t>215,456,439,600</t>
-  </si>
-  <si>
-    <t>3,941,461</t>
-  </si>
-  <si>
-    <t>233,296,941,810</t>
-  </si>
-  <si>
-    <t>53.15</t>
-  </si>
-  <si>
-    <t>53.31</t>
-  </si>
-  <si>
-    <t>53.01</t>
-  </si>
-  <si>
-    <t>-0.33điểm (-0.62 %)</t>
-  </si>
-  <si>
-    <t>26,799,134</t>
-  </si>
-  <si>
-    <t>247,055,599,600</t>
-  </si>
-  <si>
-    <t>598,859</t>
-  </si>
-  <si>
-    <t>11,903,812,900</t>
-  </si>
-  <si>
-    <t>53.48</t>
-  </si>
-  <si>
-    <t>53.61</t>
-  </si>
-  <si>
-    <t>53.11</t>
-  </si>
-  <si>
-    <t>-0.24điểm (-0.45 %)</t>
-  </si>
-  <si>
-    <t>22,960,179</t>
-  </si>
-  <si>
-    <t>297,707,086,700</t>
-  </si>
-  <si>
-    <t>76,719</t>
-  </si>
-  <si>
-    <t>2,809,190,000</t>
-  </si>
-  <si>
-    <t>53.73</t>
-  </si>
-  <si>
-    <t>53.44</t>
-  </si>
-  <si>
-    <t>53.63</t>
-  </si>
-  <si>
-    <t>0.14điểm (0.27 %)</t>
-  </si>
-  <si>
-    <t>19,483,075</t>
-  </si>
-  <si>
-    <t>254,194,013,600</t>
-  </si>
-  <si>
-    <t>1,036,090</t>
-  </si>
-  <si>
-    <t>24,788,234,000</t>
-  </si>
-  <si>
-    <t>53.49</t>
-  </si>
-  <si>
-    <t>0.59điểm (1.11 %)</t>
-  </si>
-  <si>
-    <t>24,341,876</t>
-  </si>
-  <si>
-    <t>311,148,985,800</t>
-  </si>
-  <si>
-    <t>175,141</t>
-  </si>
-  <si>
-    <t>1,768,310,000</t>
-  </si>
-  <si>
-    <t>52.90</t>
-  </si>
-  <si>
-    <t>52.91</t>
-  </si>
-  <si>
-    <t>0.54điểm (1.03 %)</t>
-  </si>
-  <si>
-    <t>31,651,876</t>
-  </si>
-  <si>
-    <t>325,625,182,700</t>
-  </si>
-  <si>
-    <t>1,851,305</t>
-  </si>
-  <si>
-    <t>50,691,392,500</t>
-  </si>
-  <si>
-    <t>52.36</t>
-  </si>
-  <si>
-    <t>53.13</t>
-  </si>
-  <si>
-    <t>52.28</t>
-  </si>
-  <si>
-    <t>52.37</t>
-  </si>
-  <si>
-    <t>0.02điểm (0.04 %)</t>
-  </si>
-  <si>
-    <t>14,613,385</t>
-  </si>
-  <si>
-    <t>213,543,324,400</t>
-  </si>
-  <si>
-    <t>881,282</t>
-  </si>
-  <si>
-    <t>23,594,070,800</t>
-  </si>
-  <si>
-    <t>52.35</t>
-  </si>
-  <si>
-    <t>52.46</t>
-  </si>
-  <si>
-    <t>52.21</t>
-  </si>
-  <si>
     <t>52.34</t>
   </si>
   <si>
@@ -1072,31 +1102,52 @@
     <t>51.71</t>
   </si>
   <si>
-    <t>04/05/2020</t>
-  </si>
-  <si>
-    <t>-0.31điểm (-0.59 %)</t>
-  </si>
-  <si>
-    <t>11,219,742</t>
-  </si>
-  <si>
-    <t>142,670,622,700</t>
-  </si>
-  <si>
-    <t>2,774,960</t>
-  </si>
-  <si>
-    <t>63,257,670,000</t>
-  </si>
-  <si>
-    <t>52.22</t>
-  </si>
-  <si>
-    <t>52.29</t>
-  </si>
-  <si>
-    <t>51.79</t>
+    <t>116.49</t>
+  </si>
+  <si>
+    <t>2.85điểm (2.50 %)</t>
+  </si>
+  <si>
+    <t>56,634,266</t>
+  </si>
+  <si>
+    <t>623,315,916,200</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>116.51</t>
+  </si>
+  <si>
+    <t>113.61</t>
+  </si>
+  <si>
+    <t>113.64</t>
+  </si>
+  <si>
+    <t>-0.49điểm (-0.43 %)</t>
+  </si>
+  <si>
+    <t>76,887,589</t>
+  </si>
+  <si>
+    <t>877,535,529,500</t>
+  </si>
+  <si>
+    <t>3,092,526</t>
+  </si>
+  <si>
+    <t>38,199,252,700</t>
+  </si>
+  <si>
+    <t>116.37</t>
+  </si>
+  <si>
+    <t>113.23</t>
   </si>
   <si>
     <t>114.14</t>
@@ -1117,9 +1168,6 @@
     <t>117,096,301,100</t>
   </si>
   <si>
-    <t>NULL</t>
-  </si>
-  <si>
     <t>114.18</t>
   </si>
   <si>
@@ -1523,54 +1571,6 @@
   </si>
   <si>
     <t>106.58</t>
-  </si>
-  <si>
-    <t>106.66</t>
-  </si>
-  <si>
-    <t>1.25điểm (1.18 %)</t>
-  </si>
-  <si>
-    <t>51,330,112</t>
-  </si>
-  <si>
-    <t>400,182,445,700</t>
-  </si>
-  <si>
-    <t>1,513,636</t>
-  </si>
-  <si>
-    <t>16,937,663,400</t>
-  </si>
-  <si>
-    <t>106.75</t>
-  </si>
-  <si>
-    <t>104.75</t>
-  </si>
-  <si>
-    <t>105.41</t>
-  </si>
-  <si>
-    <t>-0.31điểm (-0.29 %)</t>
-  </si>
-  <si>
-    <t>26,230,216</t>
-  </si>
-  <si>
-    <t>246,453,502,600</t>
-  </si>
-  <si>
-    <t>2,985,123</t>
-  </si>
-  <si>
-    <t>31,768,693,900</t>
-  </si>
-  <si>
-    <t>106.15</t>
-  </si>
-  <si>
-    <t>105.11</t>
   </si>
 </sst>
 </file>
@@ -1679,39 +1679,39 @@
         <v>18</v>
       </c>
       <c r="I2" t="s">
+        <v>12</v>
+      </c>
+      <c r="J2" t="s">
         <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" t="s">
         <v>21</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>23</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>24</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>25</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>26</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>27</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>22</v>
       </c>
       <c r="J3" t="s">
         <v>29</v>
@@ -1722,28 +1722,28 @@
         <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
         <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" t="s">
-        <v>37</v>
       </c>
       <c r="J4" t="s">
         <v>38</v>
@@ -1754,63 +1754,63 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C5" t="s">
         <v>40</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>41</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>42</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>43</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>44</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>45</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>46</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>47</v>
-      </c>
-      <c r="J5" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" t="s">
         <v>49</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>50</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>51</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>52</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>53</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>54</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>55</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>56</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>57</v>
-      </c>
-      <c r="J6" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="7">
@@ -1842,15 +1842,15 @@
         <v>66</v>
       </c>
       <c r="J7" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>67</v>
+      </c>
+      <c r="B8" t="s">
         <v>68</v>
-      </c>
-      <c r="B8" t="s">
-        <v>67</v>
       </c>
       <c r="C8" t="s">
         <v>69</v>
@@ -1882,60 +1882,60 @@
         <v>77</v>
       </c>
       <c r="B9" t="s">
+        <v>76</v>
+      </c>
+      <c r="C9" t="s">
         <v>78</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>79</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>80</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>81</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>82</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>83</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>84</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>85</v>
-      </c>
-      <c r="J9" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
+        <v>86</v>
+      </c>
+      <c r="B10" t="s">
         <v>87</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>88</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>89</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>90</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>91</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>92</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>93</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>94</v>
-      </c>
-      <c r="I10" t="s">
-        <v>88</v>
       </c>
       <c r="J10" t="s">
         <v>95</v>
@@ -1999,146 +1999,146 @@
         <v>112</v>
       </c>
       <c r="I12" t="s">
+        <v>106</v>
+      </c>
+      <c r="J12" t="s">
         <v>113</v>
-      </c>
-      <c r="J12" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" t="s">
         <v>115</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>116</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>117</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>118</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>119</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>120</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>121</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>122</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>123</v>
-      </c>
-      <c r="J13" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" t="s">
         <v>125</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>126</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>127</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>128</v>
       </c>
-      <c r="E14" t="s">
+      <c r="F14" t="s">
         <v>129</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>130</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>131</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>132</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>133</v>
-      </c>
-      <c r="J14" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" t="s">
         <v>135</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>136</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D15" t="s">
         <v>137</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>138</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>139</v>
       </c>
-      <c r="F15" t="s">
+      <c r="G15" t="s">
         <v>140</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>141</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>142</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>143</v>
-      </c>
-      <c r="J15" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>144</v>
+      </c>
+      <c r="B16" t="s">
         <v>145</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>146</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>147</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>148</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>149</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>150</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>151</v>
       </c>
-      <c r="H16" t="s">
+      <c r="I16" t="s">
         <v>152</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>153</v>
-      </c>
-      <c r="J16" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>154</v>
+      </c>
+      <c r="B17" t="s">
         <v>155</v>
-      </c>
-      <c r="B17" t="s">
-        <v>152</v>
       </c>
       <c r="C17" t="s">
         <v>156</v>
@@ -2170,28 +2170,28 @@
         <v>164</v>
       </c>
       <c r="B18" t="s">
+        <v>161</v>
+      </c>
+      <c r="C18" t="s">
         <v>165</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>166</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>167</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>168</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>169</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>170</v>
       </c>
-      <c r="H18" t="s">
+      <c r="I18" t="s">
         <v>171</v>
-      </c>
-      <c r="I18" t="s">
-        <v>165</v>
       </c>
       <c r="J18" t="s">
         <v>172</v>
@@ -2223,39 +2223,39 @@
         <v>180</v>
       </c>
       <c r="I19" t="s">
+        <v>174</v>
+      </c>
+      <c r="J19" t="s">
         <v>181</v>
-      </c>
-      <c r="J19" t="s">
-        <v>182</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>182</v>
+      </c>
+      <c r="B20" t="s">
         <v>183</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>184</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>185</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>186</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>187</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>188</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>189</v>
       </c>
-      <c r="H20" t="s">
+      <c r="I20" t="s">
         <v>190</v>
-      </c>
-      <c r="I20" t="s">
-        <v>184</v>
       </c>
       <c r="J20" t="s">
         <v>191</v>
@@ -2266,31 +2266,31 @@
         <v>192</v>
       </c>
       <c r="B21" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="C21" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" t="s">
+        <v>195</v>
+      </c>
+      <c r="E21" t="s">
+        <v>196</v>
+      </c>
+      <c r="F21" t="s">
+        <v>197</v>
+      </c>
+      <c r="G21" t="s">
+        <v>198</v>
+      </c>
+      <c r="H21" t="s">
+        <v>199</v>
+      </c>
+      <c r="I21" t="s">
         <v>193</v>
       </c>
-      <c r="D21" t="s">
-        <v>194</v>
-      </c>
-      <c r="E21" t="s">
-        <v>195</v>
-      </c>
-      <c r="F21" t="s">
-        <v>196</v>
-      </c>
-      <c r="G21" t="s">
-        <v>197</v>
-      </c>
-      <c r="H21" t="s">
-        <v>198</v>
-      </c>
-      <c r="I21" t="s">
-        <v>191</v>
-      </c>
       <c r="J21" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -2340,34 +2340,34 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="C2" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="D2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="F2" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="G2" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="H2" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="I2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3">
@@ -2375,31 +2375,31 @@
         <v>30</v>
       </c>
       <c r="B3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="C3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="D3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G3" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="I3" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="J3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4">
@@ -2407,63 +2407,63 @@
         <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="C4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="D4" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="E4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="F4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="I4" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="J4" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B5" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="C5" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="D5" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="E5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="F5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="G5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="H5" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="I5" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="J5" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
     </row>
     <row r="6">
@@ -2471,63 +2471,63 @@
         <v>58</v>
       </c>
       <c r="B6" t="s">
-        <v>233</v>
+        <v>237</v>
       </c>
       <c r="C6" t="s">
-        <v>235</v>
+        <v>238</v>
       </c>
       <c r="D6" t="s">
-        <v>236</v>
+        <v>239</v>
       </c>
       <c r="E6" t="s">
-        <v>237</v>
+        <v>240</v>
       </c>
       <c r="F6" t="s">
-        <v>238</v>
+        <v>241</v>
       </c>
       <c r="G6" t="s">
-        <v>239</v>
+        <v>242</v>
       </c>
       <c r="H6" t="s">
-        <v>224</v>
+        <v>243</v>
       </c>
       <c r="I6" t="s">
-        <v>233</v>
+        <v>244</v>
       </c>
       <c r="J6" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B7" t="s">
-        <v>227</v>
+        <v>243</v>
       </c>
       <c r="C7" t="s">
-        <v>241</v>
+        <v>202</v>
       </c>
       <c r="D7" t="s">
-        <v>242</v>
+        <v>245</v>
       </c>
       <c r="E7" t="s">
+        <v>246</v>
+      </c>
+      <c r="F7" t="s">
+        <v>247</v>
+      </c>
+      <c r="G7" t="s">
+        <v>248</v>
+      </c>
+      <c r="H7" t="s">
+        <v>234</v>
+      </c>
+      <c r="I7" t="s">
         <v>243</v>
       </c>
-      <c r="F7" t="s">
-        <v>244</v>
-      </c>
-      <c r="G7" t="s">
-        <v>245</v>
-      </c>
-      <c r="H7" t="s">
-        <v>246</v>
-      </c>
-      <c r="I7" t="s">
-        <v>227</v>
-      </c>
       <c r="J7" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
     </row>
     <row r="8">
@@ -2535,39 +2535,39 @@
         <v>77</v>
       </c>
       <c r="B8" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C8" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="D8" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="E8" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="F8" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="G8" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="H8" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="I8" t="s">
-        <v>254</v>
+        <v>237</v>
       </c>
       <c r="J8" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C9" t="s">
         <v>257</v>
@@ -2631,159 +2631,159 @@
         <v>105</v>
       </c>
       <c r="B11" t="s">
-        <v>271</v>
+        <v>274</v>
       </c>
       <c r="C11" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="D11" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E11" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="F11" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="G11" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="H11" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="I11" t="s">
-        <v>265</v>
+        <v>281</v>
       </c>
       <c r="J11" t="s">
-        <v>280</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B12" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="C12" t="s">
-        <v>281</v>
+        <v>283</v>
       </c>
       <c r="D12" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="E12" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="F12" t="s">
-        <v>284</v>
+        <v>286</v>
       </c>
       <c r="G12" t="s">
-        <v>285</v>
+        <v>287</v>
       </c>
       <c r="H12" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="I12" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="J12" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B13" t="s">
-        <v>286</v>
+        <v>288</v>
       </c>
       <c r="C13" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="D13" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E13" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="F13" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="G13" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="H13" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="I13" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="J13" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B14" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C14" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="D14" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="E14" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="F14" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="G14" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="H14" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="I14" t="s">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="J14" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C15" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="D15" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E15" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F15" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="G15" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="H15" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="I15" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="J15" t="s">
-        <v>288</v>
+        <v>312</v>
       </c>
     </row>
     <row r="16">
@@ -2791,31 +2791,31 @@
         <v>164</v>
       </c>
       <c r="B16" t="s">
-        <v>310</v>
+        <v>313</v>
       </c>
       <c r="C16" t="s">
-        <v>311</v>
+        <v>314</v>
       </c>
       <c r="D16" t="s">
-        <v>312</v>
+        <v>315</v>
       </c>
       <c r="E16" t="s">
+        <v>316</v>
+      </c>
+      <c r="F16" t="s">
+        <v>317</v>
+      </c>
+      <c r="G16" t="s">
+        <v>318</v>
+      </c>
+      <c r="H16" t="s">
+        <v>319</v>
+      </c>
+      <c r="I16" t="s">
         <v>313</v>
       </c>
-      <c r="F16" t="s">
-        <v>314</v>
-      </c>
-      <c r="G16" t="s">
-        <v>315</v>
-      </c>
-      <c r="H16" t="s">
-        <v>316</v>
-      </c>
-      <c r="I16" t="s">
-        <v>310</v>
-      </c>
       <c r="J16" t="s">
-        <v>316</v>
+        <v>297</v>
       </c>
     </row>
     <row r="17">
@@ -2823,28 +2823,28 @@
         <v>173</v>
       </c>
       <c r="B17" t="s">
-        <v>317</v>
+        <v>319</v>
       </c>
       <c r="C17" t="s">
-        <v>318</v>
+        <v>320</v>
       </c>
       <c r="D17" t="s">
+        <v>321</v>
+      </c>
+      <c r="E17" t="s">
+        <v>322</v>
+      </c>
+      <c r="F17" t="s">
+        <v>323</v>
+      </c>
+      <c r="G17" t="s">
+        <v>324</v>
+      </c>
+      <c r="H17" t="s">
+        <v>325</v>
+      </c>
+      <c r="I17" t="s">
         <v>319</v>
-      </c>
-      <c r="E17" t="s">
-        <v>320</v>
-      </c>
-      <c r="F17" t="s">
-        <v>321</v>
-      </c>
-      <c r="G17" t="s">
-        <v>322</v>
-      </c>
-      <c r="H17" t="s">
-        <v>323</v>
-      </c>
-      <c r="I17" t="s">
-        <v>324</v>
       </c>
       <c r="J17" t="s">
         <v>325</v>
@@ -2852,7 +2852,7 @@
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B18" t="s">
         <v>326</v>
@@ -2908,74 +2908,74 @@
         <v>341</v>
       </c>
       <c r="I19" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="J19" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B20" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="C20" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="D20" t="s">
+        <v>347</v>
+      </c>
+      <c r="E20" t="s">
+        <v>348</v>
+      </c>
+      <c r="F20" t="s">
+        <v>349</v>
+      </c>
+      <c r="G20" t="s">
+        <v>350</v>
+      </c>
+      <c r="H20" t="s">
+        <v>351</v>
+      </c>
+      <c r="I20" t="s">
         <v>345</v>
       </c>
-      <c r="E20" t="s">
-        <v>346</v>
-      </c>
-      <c r="F20" t="s">
-        <v>347</v>
-      </c>
-      <c r="G20" t="s">
-        <v>348</v>
-      </c>
-      <c r="H20" t="s">
-        <v>349</v>
-      </c>
-      <c r="I20" t="s">
-        <v>350</v>
-      </c>
       <c r="J20" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B21" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C21" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="D21" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="E21" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="F21" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="G21" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="H21" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="I21" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="J21" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -3025,22 +3025,22 @@
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="B2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="C2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="D2" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="E2" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="F2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="G2" t="s">
         <v>366</v>
@@ -3057,7 +3057,7 @@
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
         <v>370</v>
@@ -3089,7 +3089,7 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
         <v>378</v>
@@ -3121,7 +3121,7 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
         <v>386</v>
@@ -3153,7 +3153,7 @@
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B6" t="s">
         <v>394</v>
@@ -3185,7 +3185,7 @@
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
         <v>402</v>
@@ -3217,7 +3217,7 @@
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>77</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
         <v>410</v>
@@ -3249,7 +3249,7 @@
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
         <v>418</v>
@@ -3281,7 +3281,7 @@
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>86</v>
       </c>
       <c r="B10" t="s">
         <v>426</v>
@@ -3313,106 +3313,106 @@
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B11" t="s">
-        <v>432</v>
+        <v>434</v>
       </c>
       <c r="C11" t="s">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="D11" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="E11" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="F11" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="G11" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
       <c r="H11" t="s">
         <v>367</v>
       </c>
       <c r="I11" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="J11" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>115</v>
+        <v>105</v>
       </c>
       <c r="B12" t="s">
-        <v>393</v>
+        <v>442</v>
       </c>
       <c r="C12" t="s">
-        <v>441</v>
+        <v>443</v>
       </c>
       <c r="D12" t="s">
-        <v>442</v>
+        <v>444</v>
       </c>
       <c r="E12" t="s">
-        <v>443</v>
+        <v>445</v>
       </c>
       <c r="F12" t="s">
-        <v>444</v>
+        <v>446</v>
       </c>
       <c r="G12" t="s">
-        <v>445</v>
+        <v>447</v>
       </c>
       <c r="H12" t="s">
         <v>367</v>
       </c>
       <c r="I12" t="s">
-        <v>446</v>
+        <v>448</v>
       </c>
       <c r="J12" t="s">
-        <v>447</v>
+        <v>449</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
       <c r="B13" t="s">
         <v>448</v>
       </c>
       <c r="C13" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="D13" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="E13" t="s">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="F13" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="G13" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="H13" t="s">
         <v>367</v>
       </c>
       <c r="I13" t="s">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="J13" t="s">
-        <v>455</v>
+        <v>456</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
-        <v>456</v>
+        <v>409</v>
       </c>
       <c r="C14" t="s">
         <v>457</v>
@@ -3441,7 +3441,7 @@
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>145</v>
+        <v>134</v>
       </c>
       <c r="B15" t="s">
         <v>464</v>
@@ -3473,7 +3473,7 @@
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="B16" t="s">
         <v>472</v>
@@ -3505,7 +3505,7 @@
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>164</v>
+        <v>154</v>
       </c>
       <c r="B17" t="s">
         <v>480</v>
@@ -3529,71 +3529,71 @@
         <v>367</v>
       </c>
       <c r="I17" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="J17" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B18" t="s">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="C18" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="D18" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="E18" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="F18" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="G18" t="s">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="H18" t="s">
         <v>367</v>
       </c>
       <c r="I18" t="s">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="J18" t="s">
-        <v>494</v>
+        <v>495</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="B19" t="s">
-        <v>495</v>
+        <v>496</v>
       </c>
       <c r="C19" t="s">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="D19" t="s">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="E19" t="s">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="F19" t="s">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="G19" t="s">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="H19" t="s">
         <v>367</v>
       </c>
       <c r="I19" t="s">
-        <v>501</v>
+        <v>496</v>
       </c>
       <c r="J19" t="s">
         <v>502</v>
@@ -3601,7 +3601,7 @@
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>192</v>
+        <v>182</v>
       </c>
       <c r="B20" t="s">
         <v>503</v>
@@ -3633,7 +3633,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>343</v>
+        <v>192</v>
       </c>
       <c r="B21" t="s">
         <v>511</v>

</xml_diff>

<commit_message>
add class interface NhomChung
</commit_message>
<xml_diff>
--- a/test/stock.xlsx
+++ b/test/stock.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="516">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="515">
   <si>
     <t/>
   </si>
@@ -49,6 +49,36 @@
     <t>MinPrice</t>
   </si>
   <si>
+    <t>05/06/2020</t>
+  </si>
+  <si>
+    <t>886.22</t>
+  </si>
+  <si>
+    <t>2.32điểm (0.26 %)</t>
+  </si>
+  <si>
+    <t>443,912,540</t>
+  </si>
+  <si>
+    <t>5,179,735,000,000</t>
+  </si>
+  <si>
+    <t>32,803,881</t>
+  </si>
+  <si>
+    <t>632,309,853,760</t>
+  </si>
+  <si>
+    <t>883.40</t>
+  </si>
+  <si>
+    <t>886.59</t>
+  </si>
+  <si>
+    <t>878.50</t>
+  </si>
+  <si>
     <t>04/06/2020</t>
   </si>
   <si>
@@ -58,10 +88,10 @@
     <t>2.73điểm (0.31 %)</t>
   </si>
   <si>
-    <t>385,391,930</t>
-  </si>
-  <si>
-    <t>5,387,148,000,000</t>
+    <t>385,391,870</t>
+  </si>
+  <si>
+    <t>5,387,151,880,000</t>
   </si>
   <si>
     <t>25,330,680</t>
@@ -76,12 +106,12 @@
     <t>888.32</t>
   </si>
   <si>
+    <t>03/06/2020</t>
+  </si>
+  <si>
     <t>881.17</t>
   </si>
   <si>
-    <t>03/06/2020</t>
-  </si>
-  <si>
     <t>6.37điểm (0.73 %)</t>
   </si>
   <si>
@@ -589,453 +619,450 @@
     <t>812.48</t>
   </si>
   <si>
+    <t>56.43</t>
+  </si>
+  <si>
+    <t>0.11điểm (0.19 %)</t>
+  </si>
+  <si>
+    <t>49,185,795</t>
+  </si>
+  <si>
+    <t>506,407,438,100</t>
+  </si>
+  <si>
+    <t>1,832,920</t>
+  </si>
+  <si>
+    <t>24,505,338,400</t>
+  </si>
+  <si>
+    <t>56.33</t>
+  </si>
+  <si>
+    <t>56.51</t>
+  </si>
+  <si>
+    <t>55.99</t>
+  </si>
+  <si>
+    <t>0.00điểm (-0.01 %)</t>
+  </si>
+  <si>
+    <t>58,429,475</t>
+  </si>
+  <si>
+    <t>799,036,326,800</t>
+  </si>
+  <si>
+    <t>6,415,458</t>
+  </si>
+  <si>
+    <t>137,257,007,473</t>
+  </si>
+  <si>
+    <t>56.67</t>
+  </si>
+  <si>
+    <t>56.21</t>
+  </si>
+  <si>
+    <t>0.35điểm (0.63 %)</t>
+  </si>
+  <si>
+    <t>35,540,796</t>
+  </si>
+  <si>
+    <t>385,258,890,900</t>
+  </si>
+  <si>
+    <t>36,829,742</t>
+  </si>
+  <si>
+    <t>290,824,342,000</t>
+  </si>
+  <si>
+    <t>55.98</t>
+  </si>
+  <si>
+    <t>55.84</t>
+  </si>
+  <si>
+    <t>0.39điểm (0.71 %)</t>
+  </si>
+  <si>
+    <t>48,605,296</t>
+  </si>
+  <si>
+    <t>496,065,618,900</t>
+  </si>
+  <si>
+    <t>2,629,750</t>
+  </si>
+  <si>
+    <t>37,372,147,600</t>
+  </si>
+  <si>
+    <t>55.58</t>
+  </si>
+  <si>
+    <t>56.25</t>
+  </si>
+  <si>
+    <t>55.55</t>
+  </si>
+  <si>
+    <t>55.59</t>
+  </si>
+  <si>
+    <t>0.56điểm (1.01 %)</t>
+  </si>
+  <si>
+    <t>26,383,384</t>
+  </si>
+  <si>
+    <t>343,152,646,900</t>
+  </si>
+  <si>
+    <t>723,960</t>
+  </si>
+  <si>
+    <t>34,501,124,000</t>
+  </si>
+  <si>
+    <t>55.04</t>
+  </si>
+  <si>
+    <t>55.67</t>
+  </si>
+  <si>
+    <t>54.97</t>
+  </si>
+  <si>
+    <t>55.03</t>
+  </si>
+  <si>
+    <t>0.02điểm (0.03 %)</t>
+  </si>
+  <si>
+    <t>22,450,943</t>
+  </si>
+  <si>
+    <t>272,663,738,000</t>
+  </si>
+  <si>
+    <t>4,126,924</t>
+  </si>
+  <si>
+    <t>50,960,593,700</t>
+  </si>
+  <si>
+    <t>55.02</t>
+  </si>
+  <si>
+    <t>55.20</t>
+  </si>
+  <si>
+    <t>54.84</t>
+  </si>
+  <si>
+    <t>55.01</t>
+  </si>
+  <si>
+    <t>0.09điểm (0.16 %)</t>
+  </si>
+  <si>
+    <t>12,509,084</t>
+  </si>
+  <si>
+    <t>194,348,832,300</t>
+  </si>
+  <si>
+    <t>1,314,640</t>
+  </si>
+  <si>
+    <t>27,616,399,600</t>
+  </si>
+  <si>
+    <t>54.92</t>
+  </si>
+  <si>
+    <t>55.15</t>
+  </si>
+  <si>
+    <t>54.90</t>
+  </si>
+  <si>
+    <t>54.93</t>
+  </si>
+  <si>
+    <t>-0.40điểm (-0.72 %)</t>
+  </si>
+  <si>
+    <t>24,857,154</t>
+  </si>
+  <si>
+    <t>329,406,940,900</t>
+  </si>
+  <si>
+    <t>1,468,905</t>
+  </si>
+  <si>
+    <t>151,601,809,000</t>
+  </si>
+  <si>
+    <t>55.33</t>
+  </si>
+  <si>
+    <t>55.60</t>
+  </si>
+  <si>
+    <t>19,674,005</t>
+  </si>
+  <si>
+    <t>264,898,434,300</t>
+  </si>
+  <si>
+    <t>763,714</t>
+  </si>
+  <si>
+    <t>18,084,410,200</t>
+  </si>
+  <si>
+    <t>54.88</t>
+  </si>
+  <si>
+    <t>0.69điểm (1.28 %)</t>
+  </si>
+  <si>
+    <t>16,388,585</t>
+  </si>
+  <si>
+    <t>257,469,684,500</t>
+  </si>
+  <si>
+    <t>8,691,024</t>
+  </si>
+  <si>
+    <t>554,832,119,200</t>
+  </si>
+  <si>
+    <t>54.24</t>
+  </si>
+  <si>
+    <t>54.22</t>
+  </si>
+  <si>
+    <t>-0.07điểm (-0.13 %)</t>
+  </si>
+  <si>
+    <t>24,243,651</t>
+  </si>
+  <si>
+    <t>279,507,059,400</t>
+  </si>
+  <si>
+    <t>291,986</t>
+  </si>
+  <si>
+    <t>2,208,249,800</t>
+  </si>
+  <si>
+    <t>54.32</t>
+  </si>
+  <si>
+    <t>54.48</t>
+  </si>
+  <si>
+    <t>54.07</t>
+  </si>
+  <si>
+    <t>54.31</t>
+  </si>
+  <si>
+    <t>0.30điểm (0.55 %)</t>
+  </si>
+  <si>
+    <t>13,608,188</t>
+  </si>
+  <si>
+    <t>215,509,098,300</t>
+  </si>
+  <si>
+    <t>1,763,277</t>
+  </si>
+  <si>
+    <t>39,443,629,000</t>
+  </si>
+  <si>
+    <t>54.00</t>
+  </si>
+  <si>
+    <t>54.36</t>
+  </si>
+  <si>
+    <t>53.98</t>
+  </si>
+  <si>
+    <t>54.01</t>
+  </si>
+  <si>
+    <t>0.22điểm (0.40 %)</t>
+  </si>
+  <si>
+    <t>16,734,191</t>
+  </si>
+  <si>
+    <t>276,005,006,400</t>
+  </si>
+  <si>
+    <t>2,346,593</t>
+  </si>
+  <si>
+    <t>179,457,150,700</t>
+  </si>
+  <si>
+    <t>53.80</t>
+  </si>
+  <si>
+    <t>54.15</t>
+  </si>
+  <si>
+    <t>53.75</t>
+  </si>
+  <si>
+    <t>0.51điểm (0.96 %)</t>
+  </si>
+  <si>
+    <t>21,927,340</t>
+  </si>
+  <si>
+    <t>318,558,925,300</t>
+  </si>
+  <si>
+    <t>25,253,065</t>
+  </si>
+  <si>
+    <t>1,019,772,796,600</t>
+  </si>
+  <si>
+    <t>53.29</t>
+  </si>
+  <si>
+    <t>53.28</t>
+  </si>
+  <si>
+    <t>0.13điểm (0.25 %)</t>
+  </si>
+  <si>
+    <t>14,045,023</t>
+  </si>
+  <si>
+    <t>215,456,439,600</t>
+  </si>
+  <si>
+    <t>3,941,461</t>
+  </si>
+  <si>
+    <t>233,296,941,810</t>
+  </si>
+  <si>
+    <t>53.15</t>
+  </si>
+  <si>
+    <t>53.31</t>
+  </si>
+  <si>
+    <t>53.01</t>
+  </si>
+  <si>
+    <t>-0.33điểm (-0.62 %)</t>
+  </si>
+  <si>
+    <t>26,799,134</t>
+  </si>
+  <si>
+    <t>247,055,599,600</t>
+  </si>
+  <si>
+    <t>598,859</t>
+  </si>
+  <si>
+    <t>11,903,812,900</t>
+  </si>
+  <si>
+    <t>53.48</t>
+  </si>
+  <si>
+    <t>53.61</t>
+  </si>
+  <si>
+    <t>53.11</t>
+  </si>
+  <si>
+    <t>-0.24điểm (-0.45 %)</t>
+  </si>
+  <si>
+    <t>22,960,179</t>
+  </si>
+  <si>
+    <t>297,707,086,700</t>
+  </si>
+  <si>
+    <t>76,719</t>
+  </si>
+  <si>
+    <t>2,809,190,000</t>
+  </si>
+  <si>
+    <t>53.73</t>
+  </si>
+  <si>
+    <t>53.44</t>
+  </si>
+  <si>
+    <t>53.63</t>
+  </si>
+  <si>
+    <t>0.14điểm (0.27 %)</t>
+  </si>
+  <si>
+    <t>19,483,075</t>
+  </si>
+  <si>
+    <t>254,194,013,600</t>
+  </si>
+  <si>
+    <t>1,036,090</t>
+  </si>
+  <si>
+    <t>24,788,234,000</t>
+  </si>
+  <si>
+    <t>53.49</t>
+  </si>
+  <si>
+    <t>0.59điểm (1.11 %)</t>
+  </si>
+  <si>
+    <t>24,341,876</t>
+  </si>
+  <si>
+    <t>311,148,985,800</t>
+  </si>
+  <si>
+    <t>175,141</t>
+  </si>
+  <si>
+    <t>1,768,310,000</t>
+  </si>
+  <si>
+    <t>52.90</t>
+  </si>
+  <si>
     <t>08/05/2020</t>
   </si>
   <si>
-    <t>813.73</t>
-  </si>
-  <si>
-    <t>17.19điểm (2.16 %)</t>
-  </si>
-  <si>
-    <t>327,812,460</t>
-  </si>
-  <si>
-    <t>6,274,440,880,000</t>
-  </si>
-  <si>
-    <t>28,819,969</t>
-  </si>
-  <si>
-    <t>672,193,589,050</t>
-  </si>
-  <si>
-    <t>800.32</t>
-  </si>
-  <si>
-    <t>825.72</t>
-  </si>
-  <si>
-    <t>800.20</t>
-  </si>
-  <si>
-    <t>56.33</t>
-  </si>
-  <si>
-    <t>0.00điểm (-0.01 %)</t>
-  </si>
-  <si>
-    <t>58,429,475</t>
-  </si>
-  <si>
-    <t>799,036,326,800</t>
-  </si>
-  <si>
-    <t>5,961,458</t>
-  </si>
-  <si>
-    <t>129,085,007,473</t>
-  </si>
-  <si>
-    <t>56.67</t>
-  </si>
-  <si>
-    <t>56.21</t>
-  </si>
-  <si>
-    <t>0.35điểm (0.63 %)</t>
-  </si>
-  <si>
-    <t>35,540,796</t>
-  </si>
-  <si>
-    <t>385,258,890,900</t>
-  </si>
-  <si>
-    <t>36,829,742</t>
-  </si>
-  <si>
-    <t>290,824,342,000</t>
-  </si>
-  <si>
-    <t>55.98</t>
-  </si>
-  <si>
-    <t>55.84</t>
-  </si>
-  <si>
-    <t>0.39điểm (0.71 %)</t>
-  </si>
-  <si>
-    <t>48,605,296</t>
-  </si>
-  <si>
-    <t>496,065,618,900</t>
-  </si>
-  <si>
-    <t>2,629,750</t>
-  </si>
-  <si>
-    <t>37,372,147,600</t>
-  </si>
-  <si>
-    <t>55.58</t>
-  </si>
-  <si>
-    <t>56.25</t>
-  </si>
-  <si>
-    <t>55.55</t>
-  </si>
-  <si>
-    <t>55.59</t>
-  </si>
-  <si>
-    <t>0.56điểm (1.01 %)</t>
-  </si>
-  <si>
-    <t>26,383,384</t>
-  </si>
-  <si>
-    <t>343,152,646,900</t>
-  </si>
-  <si>
-    <t>723,960</t>
-  </si>
-  <si>
-    <t>34,501,124,000</t>
-  </si>
-  <si>
-    <t>55.04</t>
-  </si>
-  <si>
-    <t>55.67</t>
-  </si>
-  <si>
-    <t>54.97</t>
-  </si>
-  <si>
-    <t>55.03</t>
-  </si>
-  <si>
-    <t>0.02điểm (0.03 %)</t>
-  </si>
-  <si>
-    <t>22,450,943</t>
-  </si>
-  <si>
-    <t>272,663,738,000</t>
-  </si>
-  <si>
-    <t>4,126,924</t>
-  </si>
-  <si>
-    <t>50,960,593,700</t>
-  </si>
-  <si>
-    <t>55.02</t>
-  </si>
-  <si>
-    <t>55.20</t>
-  </si>
-  <si>
-    <t>54.84</t>
-  </si>
-  <si>
-    <t>55.01</t>
-  </si>
-  <si>
-    <t>0.09điểm (0.16 %)</t>
-  </si>
-  <si>
-    <t>12,509,084</t>
-  </si>
-  <si>
-    <t>194,348,832,300</t>
-  </si>
-  <si>
-    <t>1,314,640</t>
-  </si>
-  <si>
-    <t>27,616,399,600</t>
-  </si>
-  <si>
-    <t>54.92</t>
-  </si>
-  <si>
-    <t>55.15</t>
-  </si>
-  <si>
-    <t>54.90</t>
-  </si>
-  <si>
-    <t>54.93</t>
-  </si>
-  <si>
-    <t>-0.40điểm (-0.72 %)</t>
-  </si>
-  <si>
-    <t>24,857,154</t>
-  </si>
-  <si>
-    <t>329,406,940,900</t>
-  </si>
-  <si>
-    <t>1,468,905</t>
-  </si>
-  <si>
-    <t>151,601,809,000</t>
-  </si>
-  <si>
-    <t>55.33</t>
-  </si>
-  <si>
-    <t>55.60</t>
-  </si>
-  <si>
-    <t>19,674,005</t>
-  </si>
-  <si>
-    <t>264,898,434,300</t>
-  </si>
-  <si>
-    <t>763,714</t>
-  </si>
-  <si>
-    <t>18,084,410,200</t>
-  </si>
-  <si>
-    <t>54.88</t>
-  </si>
-  <si>
-    <t>0.69điểm (1.28 %)</t>
-  </si>
-  <si>
-    <t>16,388,585</t>
-  </si>
-  <si>
-    <t>257,469,684,500</t>
-  </si>
-  <si>
-    <t>8,691,024</t>
-  </si>
-  <si>
-    <t>554,832,119,200</t>
-  </si>
-  <si>
-    <t>54.24</t>
-  </si>
-  <si>
-    <t>54.22</t>
-  </si>
-  <si>
-    <t>-0.07điểm (-0.13 %)</t>
-  </si>
-  <si>
-    <t>24,243,651</t>
-  </si>
-  <si>
-    <t>279,507,059,400</t>
-  </si>
-  <si>
-    <t>291,986</t>
-  </si>
-  <si>
-    <t>2,208,249,800</t>
-  </si>
-  <si>
-    <t>54.32</t>
-  </si>
-  <si>
-    <t>54.48</t>
-  </si>
-  <si>
-    <t>54.07</t>
-  </si>
-  <si>
-    <t>54.31</t>
-  </si>
-  <si>
-    <t>0.30điểm (0.55 %)</t>
-  </si>
-  <si>
-    <t>13,608,188</t>
-  </si>
-  <si>
-    <t>215,509,098,300</t>
-  </si>
-  <si>
-    <t>1,763,277</t>
-  </si>
-  <si>
-    <t>39,443,629,000</t>
-  </si>
-  <si>
-    <t>54.00</t>
-  </si>
-  <si>
-    <t>54.36</t>
-  </si>
-  <si>
-    <t>53.98</t>
-  </si>
-  <si>
-    <t>54.01</t>
-  </si>
-  <si>
-    <t>0.22điểm (0.40 %)</t>
-  </si>
-  <si>
-    <t>16,734,191</t>
-  </si>
-  <si>
-    <t>276,005,006,400</t>
-  </si>
-  <si>
-    <t>2,346,593</t>
-  </si>
-  <si>
-    <t>179,457,150,700</t>
-  </si>
-  <si>
-    <t>53.80</t>
-  </si>
-  <si>
-    <t>54.15</t>
-  </si>
-  <si>
-    <t>53.75</t>
-  </si>
-  <si>
-    <t>0.51điểm (0.96 %)</t>
-  </si>
-  <si>
-    <t>21,927,340</t>
-  </si>
-  <si>
-    <t>318,558,925,300</t>
-  </si>
-  <si>
-    <t>25,253,065</t>
-  </si>
-  <si>
-    <t>1,019,772,796,600</t>
-  </si>
-  <si>
-    <t>53.29</t>
-  </si>
-  <si>
-    <t>53.28</t>
-  </si>
-  <si>
-    <t>0.13điểm (0.25 %)</t>
-  </si>
-  <si>
-    <t>14,045,023</t>
-  </si>
-  <si>
-    <t>215,456,439,600</t>
-  </si>
-  <si>
-    <t>3,941,461</t>
-  </si>
-  <si>
-    <t>233,296,941,810</t>
-  </si>
-  <si>
-    <t>53.15</t>
-  </si>
-  <si>
-    <t>53.31</t>
-  </si>
-  <si>
-    <t>53.01</t>
-  </si>
-  <si>
-    <t>-0.33điểm (-0.62 %)</t>
-  </si>
-  <si>
-    <t>26,799,134</t>
-  </si>
-  <si>
-    <t>247,055,599,600</t>
-  </si>
-  <si>
-    <t>598,859</t>
-  </si>
-  <si>
-    <t>11,903,812,900</t>
-  </si>
-  <si>
-    <t>53.48</t>
-  </si>
-  <si>
-    <t>53.61</t>
-  </si>
-  <si>
-    <t>53.11</t>
-  </si>
-  <si>
-    <t>-0.24điểm (-0.45 %)</t>
-  </si>
-  <si>
-    <t>22,960,179</t>
-  </si>
-  <si>
-    <t>297,707,086,700</t>
-  </si>
-  <si>
-    <t>76,719</t>
-  </si>
-  <si>
-    <t>2,809,190,000</t>
-  </si>
-  <si>
-    <t>53.73</t>
-  </si>
-  <si>
-    <t>53.44</t>
-  </si>
-  <si>
-    <t>53.63</t>
-  </si>
-  <si>
-    <t>0.14điểm (0.27 %)</t>
-  </si>
-  <si>
-    <t>19,483,075</t>
-  </si>
-  <si>
-    <t>254,194,013,600</t>
-  </si>
-  <si>
-    <t>1,036,090</t>
-  </si>
-  <si>
-    <t>24,788,234,000</t>
-  </si>
-  <si>
-    <t>53.49</t>
-  </si>
-  <si>
-    <t>0.59điểm (1.11 %)</t>
-  </si>
-  <si>
-    <t>24,341,876</t>
-  </si>
-  <si>
-    <t>311,148,985,800</t>
-  </si>
-  <si>
-    <t>175,141</t>
-  </si>
-  <si>
-    <t>1,768,310,000</t>
-  </si>
-  <si>
-    <t>52.90</t>
-  </si>
-  <si>
     <t>52.91</t>
   </si>
   <si>
@@ -1063,34 +1090,28 @@
     <t>52.28</t>
   </si>
   <si>
-    <t>07/05/2020</t>
-  </si>
-  <si>
-    <t>52.37</t>
-  </si>
-  <si>
-    <t>0.02điểm (0.04 %)</t>
-  </si>
-  <si>
-    <t>14,613,385</t>
-  </si>
-  <si>
-    <t>213,543,324,400</t>
-  </si>
-  <si>
-    <t>881,282</t>
-  </si>
-  <si>
-    <t>23,594,070,800</t>
-  </si>
-  <si>
-    <t>52.35</t>
-  </si>
-  <si>
-    <t>52.46</t>
-  </si>
-  <si>
-    <t>52.21</t>
+    <t>118.08</t>
+  </si>
+  <si>
+    <t>0.66điểm (0.56 %)</t>
+  </si>
+  <si>
+    <t>67,376,517</t>
+  </si>
+  <si>
+    <t>721,127,276,800</t>
+  </si>
+  <si>
+    <t>2,431,877</t>
+  </si>
+  <si>
+    <t>43,136,829,900</t>
+  </si>
+  <si>
+    <t>NULL</t>
+  </si>
+  <si>
+    <t>116.35</t>
   </si>
   <si>
     <t>117.42</t>
@@ -1105,10 +1126,10 @@
     <t>682,544,489,600</t>
   </si>
   <si>
-    <t>0</t>
-  </si>
-  <si>
-    <t>NULL</t>
+    <t>17,953,802</t>
+  </si>
+  <si>
+    <t>284,497,267,600</t>
   </si>
   <si>
     <t>117.89</t>
@@ -1538,30 +1559,6 @@
   </si>
   <si>
     <t>110.03</t>
-  </si>
-  <si>
-    <t>110.02</t>
-  </si>
-  <si>
-    <t>1.71điểm (1.58 %)</t>
-  </si>
-  <si>
-    <t>62,052,998</t>
-  </si>
-  <si>
-    <t>544,818,404,000</t>
-  </si>
-  <si>
-    <t>3,462,992</t>
-  </si>
-  <si>
-    <t>21,275,023,700</t>
-  </si>
-  <si>
-    <t>110.79</t>
-  </si>
-  <si>
-    <t>107.20</t>
   </si>
 </sst>
 </file>
@@ -1681,28 +1678,28 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="H3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="J3" t="s">
         <v>28</v>
@@ -1710,31 +1707,31 @@
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C4" t="s">
+        <v>32</v>
+      </c>
+      <c r="D4" t="s">
+        <v>33</v>
+      </c>
+      <c r="E4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F4" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I4" t="s">
         <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>32</v>
-      </c>
-      <c r="E4" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G4" t="s">
-        <v>35</v>
-      </c>
-      <c r="H4" t="s">
-        <v>36</v>
-      </c>
-      <c r="I4" t="s">
-        <v>37</v>
       </c>
       <c r="J4" t="s">
         <v>38</v>
@@ -1766,50 +1763,50 @@
         <v>46</v>
       </c>
       <c r="I5" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="J5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="C6" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" t="s">
+        <v>56</v>
+      </c>
+      <c r="I6" t="s">
         <v>50</v>
       </c>
-      <c r="E6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G6" t="s">
-        <v>53</v>
-      </c>
-      <c r="H6" t="s">
-        <v>54</v>
-      </c>
-      <c r="I6" t="s">
-        <v>55</v>
-      </c>
       <c r="J6" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
         <v>57</v>
-      </c>
-      <c r="B7" t="s">
-        <v>58</v>
       </c>
       <c r="C7" t="s">
         <v>59</v>
@@ -1865,39 +1862,39 @@
         <v>75</v>
       </c>
       <c r="J8" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D9" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" t="s">
+        <v>82</v>
+      </c>
+      <c r="G9" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" t="s">
+        <v>84</v>
+      </c>
+      <c r="I9" t="s">
+        <v>85</v>
+      </c>
+      <c r="J9" t="s">
         <v>78</v>
-      </c>
-      <c r="D9" t="s">
-        <v>79</v>
-      </c>
-      <c r="E9" t="s">
-        <v>80</v>
-      </c>
-      <c r="F9" t="s">
-        <v>81</v>
-      </c>
-      <c r="G9" t="s">
-        <v>82</v>
-      </c>
-      <c r="H9" t="s">
-        <v>83</v>
-      </c>
-      <c r="I9" t="s">
-        <v>84</v>
-      </c>
-      <c r="J9" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="10">
@@ -1905,39 +1902,39 @@
         <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D10" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="E10" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="F10" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="G10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="H10" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="I10" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="J10" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B11" t="s">
         <v>95</v>
-      </c>
-      <c r="B11" t="s">
-        <v>96</v>
       </c>
       <c r="C11" t="s">
         <v>97</v>
@@ -1990,71 +1987,71 @@
         <v>112</v>
       </c>
       <c r="I12" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="J12" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C13" t="s">
+        <v>117</v>
+      </c>
+      <c r="D13" t="s">
+        <v>118</v>
+      </c>
+      <c r="E13" t="s">
+        <v>119</v>
+      </c>
+      <c r="F13" t="s">
+        <v>120</v>
+      </c>
+      <c r="G13" t="s">
+        <v>121</v>
+      </c>
+      <c r="H13" t="s">
+        <v>122</v>
+      </c>
+      <c r="I13" t="s">
         <v>116</v>
       </c>
-      <c r="D13" t="s">
-        <v>117</v>
-      </c>
-      <c r="E13" t="s">
-        <v>118</v>
-      </c>
-      <c r="F13" t="s">
-        <v>119</v>
-      </c>
-      <c r="G13" t="s">
-        <v>120</v>
-      </c>
-      <c r="H13" t="s">
-        <v>121</v>
-      </c>
-      <c r="I13" t="s">
-        <v>115</v>
-      </c>
       <c r="J13" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C14" t="s">
+        <v>126</v>
+      </c>
+      <c r="D14" t="s">
+        <v>127</v>
+      </c>
+      <c r="E14" t="s">
+        <v>128</v>
+      </c>
+      <c r="F14" t="s">
+        <v>129</v>
+      </c>
+      <c r="G14" t="s">
+        <v>130</v>
+      </c>
+      <c r="H14" t="s">
+        <v>131</v>
+      </c>
+      <c r="I14" t="s">
         <v>125</v>
-      </c>
-      <c r="D14" t="s">
-        <v>126</v>
-      </c>
-      <c r="E14" t="s">
-        <v>127</v>
-      </c>
-      <c r="F14" t="s">
-        <v>128</v>
-      </c>
-      <c r="G14" t="s">
-        <v>129</v>
-      </c>
-      <c r="H14" t="s">
-        <v>130</v>
-      </c>
-      <c r="I14" t="s">
-        <v>131</v>
       </c>
       <c r="J14" t="s">
         <v>132</v>
@@ -2193,39 +2190,39 @@
         <v>173</v>
       </c>
       <c r="B19" t="s">
-        <v>170</v>
+        <v>174</v>
       </c>
       <c r="C19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="D19" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="E19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="F19" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="G19" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="H19" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="I19" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="J19" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B20" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C20" t="s">
         <v>184</v>
@@ -2246,39 +2243,39 @@
         <v>189</v>
       </c>
       <c r="I20" t="s">
-        <v>183</v>
+        <v>190</v>
       </c>
       <c r="J20" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B21" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="C21" t="s">
+        <v>194</v>
+      </c>
+      <c r="D21" t="s">
+        <v>195</v>
+      </c>
+      <c r="E21" t="s">
+        <v>196</v>
+      </c>
+      <c r="F21" t="s">
+        <v>197</v>
+      </c>
+      <c r="G21" t="s">
+        <v>198</v>
+      </c>
+      <c r="H21" t="s">
+        <v>199</v>
+      </c>
+      <c r="I21" t="s">
         <v>193</v>
-      </c>
-      <c r="D21" t="s">
-        <v>194</v>
-      </c>
-      <c r="E21" t="s">
-        <v>195</v>
-      </c>
-      <c r="F21" t="s">
-        <v>196</v>
-      </c>
-      <c r="G21" t="s">
-        <v>197</v>
-      </c>
-      <c r="H21" t="s">
-        <v>198</v>
-      </c>
-      <c r="I21" t="s">
-        <v>199</v>
       </c>
       <c r="J21" t="s">
         <v>200</v>
@@ -2352,13 +2349,13 @@
         <v>206</v>
       </c>
       <c r="H2" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="I2" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="J2" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
     </row>
     <row r="3">
@@ -2366,60 +2363,60 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>201</v>
+        <v>207</v>
       </c>
       <c r="C3" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="D3" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="E3" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="F3" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="G3" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="H3" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="I3" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="J3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
+        <v>207</v>
       </c>
       <c r="C4" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="D4" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E4" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="F4" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="G4" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="H4" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="I4" t="s">
-        <v>222</v>
+        <v>207</v>
       </c>
       <c r="J4" t="s">
         <v>223</v>
@@ -2430,95 +2427,95 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
+        <v>222</v>
+      </c>
+      <c r="C5" t="s">
         <v>224</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>225</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>226</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>227</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>228</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>229</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>230</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>231</v>
-      </c>
-      <c r="J5" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
+        <v>232</v>
+      </c>
+      <c r="C6" t="s">
         <v>233</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>234</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>235</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>236</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>237</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>238</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>239</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>240</v>
-      </c>
-      <c r="J6" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
+        <v>241</v>
+      </c>
+      <c r="C7" t="s">
         <v>242</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>243</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>244</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>245</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>246</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>247</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>248</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>249</v>
-      </c>
-      <c r="J7" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="8">
@@ -2526,63 +2523,63 @@
         <v>67</v>
       </c>
       <c r="B8" t="s">
+        <v>250</v>
+      </c>
+      <c r="C8" t="s">
         <v>251</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>252</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>253</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>254</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>255</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>256</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>257</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>258</v>
-      </c>
-      <c r="J8" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C9" t="s">
-        <v>216</v>
+        <v>260</v>
       </c>
       <c r="D9" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="E9" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="F9" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="G9" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="H9" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="I9" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
       <c r="J9" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10">
@@ -2590,60 +2587,60 @@
         <v>86</v>
       </c>
       <c r="B10" t="s">
-        <v>251</v>
+        <v>265</v>
       </c>
       <c r="C10" t="s">
-        <v>264</v>
+        <v>224</v>
       </c>
       <c r="D10" t="s">
+        <v>267</v>
+      </c>
+      <c r="E10" t="s">
+        <v>268</v>
+      </c>
+      <c r="F10" t="s">
+        <v>269</v>
+      </c>
+      <c r="G10" t="s">
+        <v>270</v>
+      </c>
+      <c r="H10" t="s">
+        <v>256</v>
+      </c>
+      <c r="I10" t="s">
         <v>265</v>
       </c>
-      <c r="E10" t="s">
-        <v>266</v>
-      </c>
-      <c r="F10" t="s">
-        <v>267</v>
-      </c>
-      <c r="G10" t="s">
-        <v>268</v>
-      </c>
-      <c r="H10" t="s">
-        <v>269</v>
-      </c>
-      <c r="I10" t="s">
-        <v>251</v>
-      </c>
       <c r="J10" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B11" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="C11" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="D11" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="E11" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="F11" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="G11" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="H11" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="I11" t="s">
-        <v>277</v>
+        <v>259</v>
       </c>
       <c r="J11" t="s">
         <v>278</v>
@@ -2654,71 +2651,71 @@
         <v>105</v>
       </c>
       <c r="B12" t="s">
+        <v>277</v>
+      </c>
+      <c r="C12" t="s">
         <v>279</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>280</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>281</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>282</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>283</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>284</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>285</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>286</v>
-      </c>
-      <c r="J12" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B13" t="s">
+        <v>287</v>
+      </c>
+      <c r="C13" t="s">
         <v>288</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>289</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>290</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>291</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>292</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>293</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>294</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>295</v>
-      </c>
-      <c r="J13" t="s">
-        <v>296</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
-        <v>294</v>
+        <v>296</v>
       </c>
       <c r="C14" t="s">
         <v>297</v>
@@ -2739,10 +2736,10 @@
         <v>302</v>
       </c>
       <c r="I14" t="s">
-        <v>288</v>
+        <v>303</v>
       </c>
       <c r="J14" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
     </row>
     <row r="15">
@@ -2753,25 +2750,25 @@
         <v>302</v>
       </c>
       <c r="C15" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="D15" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="E15" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="F15" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G15" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H15" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="I15" t="s">
-        <v>310</v>
+        <v>296</v>
       </c>
       <c r="J15" t="s">
         <v>311</v>
@@ -2782,7 +2779,7 @@
         <v>143</v>
       </c>
       <c r="B16" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="C16" t="s">
         <v>312</v>
@@ -2835,18 +2832,18 @@
         <v>325</v>
       </c>
       <c r="I17" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="J17" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>173</v>
+        <v>163</v>
       </c>
       <c r="B18" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C18" t="s">
         <v>328</v>
@@ -2867,106 +2864,106 @@
         <v>333</v>
       </c>
       <c r="I18" t="s">
-        <v>327</v>
+        <v>333</v>
       </c>
       <c r="J18" t="s">
-        <v>311</v>
+        <v>334</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B19" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C19" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="D19" t="s">
+        <v>337</v>
+      </c>
+      <c r="E19" t="s">
+        <v>338</v>
+      </c>
+      <c r="F19" t="s">
+        <v>339</v>
+      </c>
+      <c r="G19" t="s">
+        <v>340</v>
+      </c>
+      <c r="H19" t="s">
+        <v>341</v>
+      </c>
+      <c r="I19" t="s">
         <v>335</v>
       </c>
-      <c r="E19" t="s">
-        <v>336</v>
-      </c>
-      <c r="F19" t="s">
-        <v>337</v>
-      </c>
-      <c r="G19" t="s">
-        <v>338</v>
-      </c>
-      <c r="H19" t="s">
-        <v>339</v>
-      </c>
-      <c r="I19" t="s">
-        <v>333</v>
-      </c>
       <c r="J19" t="s">
-        <v>339</v>
+        <v>319</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B20" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="C20" t="s">
+        <v>342</v>
+      </c>
+      <c r="D20" t="s">
+        <v>343</v>
+      </c>
+      <c r="E20" t="s">
+        <v>344</v>
+      </c>
+      <c r="F20" t="s">
+        <v>345</v>
+      </c>
+      <c r="G20" t="s">
+        <v>346</v>
+      </c>
+      <c r="H20" t="s">
+        <v>347</v>
+      </c>
+      <c r="I20" t="s">
         <v>341</v>
       </c>
-      <c r="D20" t="s">
-        <v>342</v>
-      </c>
-      <c r="E20" t="s">
-        <v>343</v>
-      </c>
-      <c r="F20" t="s">
-        <v>344</v>
-      </c>
-      <c r="G20" t="s">
-        <v>345</v>
-      </c>
-      <c r="H20" t="s">
-        <v>346</v>
-      </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>347</v>
-      </c>
-      <c r="J20" t="s">
-        <v>348</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
+        <v>348</v>
+      </c>
+      <c r="B21" t="s">
         <v>349</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>350</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>351</v>
       </c>
-      <c r="D21" t="s">
+      <c r="E21" t="s">
         <v>352</v>
       </c>
-      <c r="E21" t="s">
+      <c r="F21" t="s">
         <v>353</v>
       </c>
-      <c r="F21" t="s">
+      <c r="G21" t="s">
         <v>354</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>355</v>
       </c>
-      <c r="H21" t="s">
+      <c r="I21" t="s">
         <v>356</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>357</v>
-      </c>
-      <c r="J21" t="s">
-        <v>358</v>
       </c>
     </row>
   </sheetData>
@@ -3019,19 +3016,19 @@
         <v>11</v>
       </c>
       <c r="B2" t="s">
+        <v>358</v>
+      </c>
+      <c r="C2" t="s">
         <v>359</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>360</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>361</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>362</v>
-      </c>
-      <c r="F2" t="s">
-        <v>363</v>
       </c>
       <c r="G2" t="s">
         <v>363</v>
@@ -3040,10 +3037,10 @@
         <v>364</v>
       </c>
       <c r="I2" t="s">
+        <v>358</v>
+      </c>
+      <c r="J2" t="s">
         <v>365</v>
-      </c>
-      <c r="J2" t="s">
-        <v>366</v>
       </c>
     </row>
     <row r="3">
@@ -3051,63 +3048,63 @@
         <v>21</v>
       </c>
       <c r="B3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C3" t="s">
         <v>367</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>368</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>369</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>370</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>371</v>
-      </c>
-      <c r="G3" t="s">
-        <v>372</v>
       </c>
       <c r="H3" t="s">
         <v>364</v>
       </c>
       <c r="I3" t="s">
+        <v>372</v>
+      </c>
+      <c r="J3" t="s">
         <v>373</v>
-      </c>
-      <c r="J3" t="s">
-        <v>374</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B4" t="s">
+        <v>374</v>
+      </c>
+      <c r="C4" t="s">
         <v>375</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>376</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>377</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>378</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>379</v>
-      </c>
-      <c r="G4" t="s">
-        <v>380</v>
       </c>
       <c r="H4" t="s">
         <v>364</v>
       </c>
       <c r="I4" t="s">
+        <v>380</v>
+      </c>
+      <c r="J4" t="s">
         <v>381</v>
-      </c>
-      <c r="J4" t="s">
-        <v>382</v>
       </c>
     </row>
     <row r="5">
@@ -3115,95 +3112,95 @@
         <v>39</v>
       </c>
       <c r="B5" t="s">
+        <v>382</v>
+      </c>
+      <c r="C5" t="s">
         <v>383</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>384</v>
       </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>385</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>386</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>387</v>
-      </c>
-      <c r="G5" t="s">
-        <v>388</v>
       </c>
       <c r="H5" t="s">
         <v>364</v>
       </c>
       <c r="I5" t="s">
+        <v>388</v>
+      </c>
+      <c r="J5" t="s">
         <v>389</v>
-      </c>
-      <c r="J5" t="s">
-        <v>390</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B6" t="s">
+        <v>390</v>
+      </c>
+      <c r="C6" t="s">
         <v>391</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>392</v>
       </c>
-      <c r="D6" t="s">
+      <c r="E6" t="s">
         <v>393</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>394</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>395</v>
-      </c>
-      <c r="G6" t="s">
-        <v>396</v>
       </c>
       <c r="H6" t="s">
         <v>364</v>
       </c>
       <c r="I6" t="s">
+        <v>396</v>
+      </c>
+      <c r="J6" t="s">
         <v>397</v>
-      </c>
-      <c r="J6" t="s">
-        <v>398</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B7" t="s">
+        <v>398</v>
+      </c>
+      <c r="C7" t="s">
         <v>399</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>400</v>
       </c>
-      <c r="D7" t="s">
+      <c r="E7" t="s">
         <v>401</v>
       </c>
-      <c r="E7" t="s">
+      <c r="F7" t="s">
         <v>402</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>403</v>
-      </c>
-      <c r="G7" t="s">
-        <v>404</v>
       </c>
       <c r="H7" t="s">
         <v>364</v>
       </c>
       <c r="I7" t="s">
+        <v>404</v>
+      </c>
+      <c r="J7" t="s">
         <v>405</v>
-      </c>
-      <c r="J7" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="8">
@@ -3211,63 +3208,63 @@
         <v>67</v>
       </c>
       <c r="B8" t="s">
+        <v>406</v>
+      </c>
+      <c r="C8" t="s">
         <v>407</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>408</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>409</v>
       </c>
-      <c r="E8" t="s">
+      <c r="F8" t="s">
         <v>410</v>
       </c>
-      <c r="F8" t="s">
+      <c r="G8" t="s">
         <v>411</v>
-      </c>
-      <c r="G8" t="s">
-        <v>412</v>
       </c>
       <c r="H8" t="s">
         <v>364</v>
       </c>
       <c r="I8" t="s">
+        <v>412</v>
+      </c>
+      <c r="J8" t="s">
         <v>413</v>
-      </c>
-      <c r="J8" t="s">
-        <v>414</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
+        <v>414</v>
+      </c>
+      <c r="C9" t="s">
         <v>415</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>416</v>
       </c>
-      <c r="D9" t="s">
+      <c r="E9" t="s">
         <v>417</v>
       </c>
-      <c r="E9" t="s">
+      <c r="F9" t="s">
         <v>418</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>419</v>
-      </c>
-      <c r="G9" t="s">
-        <v>420</v>
       </c>
       <c r="H9" t="s">
         <v>364</v>
       </c>
       <c r="I9" t="s">
+        <v>420</v>
+      </c>
+      <c r="J9" t="s">
         <v>421</v>
-      </c>
-      <c r="J9" t="s">
-        <v>422</v>
       </c>
     </row>
     <row r="10">
@@ -3275,63 +3272,63 @@
         <v>86</v>
       </c>
       <c r="B10" t="s">
+        <v>422</v>
+      </c>
+      <c r="C10" t="s">
         <v>423</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>424</v>
       </c>
-      <c r="D10" t="s">
+      <c r="E10" t="s">
         <v>425</v>
       </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
         <v>426</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>427</v>
-      </c>
-      <c r="G10" t="s">
-        <v>428</v>
       </c>
       <c r="H10" t="s">
         <v>364</v>
       </c>
       <c r="I10" t="s">
+        <v>428</v>
+      </c>
+      <c r="J10" t="s">
         <v>429</v>
-      </c>
-      <c r="J10" t="s">
-        <v>430</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B11" t="s">
+        <v>430</v>
+      </c>
+      <c r="C11" t="s">
         <v>431</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>432</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>433</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>434</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>435</v>
-      </c>
-      <c r="G11" t="s">
-        <v>436</v>
       </c>
       <c r="H11" t="s">
         <v>364</v>
       </c>
       <c r="I11" t="s">
+        <v>436</v>
+      </c>
+      <c r="J11" t="s">
         <v>437</v>
-      </c>
-      <c r="J11" t="s">
-        <v>438</v>
       </c>
     </row>
     <row r="12">
@@ -3339,71 +3336,71 @@
         <v>105</v>
       </c>
       <c r="B12" t="s">
+        <v>438</v>
+      </c>
+      <c r="C12" t="s">
         <v>439</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>440</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>441</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>442</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>443</v>
-      </c>
-      <c r="G12" t="s">
-        <v>444</v>
       </c>
       <c r="H12" t="s">
         <v>364</v>
       </c>
       <c r="I12" t="s">
+        <v>444</v>
+      </c>
+      <c r="J12" t="s">
         <v>445</v>
-      </c>
-      <c r="J12" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B13" t="s">
+        <v>446</v>
+      </c>
+      <c r="C13" t="s">
         <v>447</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>448</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>449</v>
       </c>
-      <c r="E13" t="s">
+      <c r="F13" t="s">
         <v>450</v>
       </c>
-      <c r="F13" t="s">
+      <c r="G13" t="s">
         <v>451</v>
-      </c>
-      <c r="G13" t="s">
-        <v>452</v>
       </c>
       <c r="H13" t="s">
         <v>364</v>
       </c>
       <c r="I13" t="s">
+        <v>452</v>
+      </c>
+      <c r="J13" t="s">
         <v>453</v>
-      </c>
-      <c r="J13" t="s">
-        <v>454</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B14" t="s">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C14" t="s">
         <v>455</v>
@@ -3435,7 +3432,7 @@
         <v>133</v>
       </c>
       <c r="B15" t="s">
-        <v>414</v>
+        <v>460</v>
       </c>
       <c r="C15" t="s">
         <v>462</v>
@@ -3467,31 +3464,31 @@
         <v>143</v>
       </c>
       <c r="B16" t="s">
+        <v>421</v>
+      </c>
+      <c r="C16" t="s">
         <v>469</v>
       </c>
-      <c r="C16" t="s">
+      <c r="D16" t="s">
         <v>470</v>
       </c>
-      <c r="D16" t="s">
+      <c r="E16" t="s">
         <v>471</v>
       </c>
-      <c r="E16" t="s">
+      <c r="F16" t="s">
         <v>472</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>473</v>
-      </c>
-      <c r="G16" t="s">
-        <v>474</v>
       </c>
       <c r="H16" t="s">
         <v>364</v>
       </c>
       <c r="I16" t="s">
+        <v>474</v>
+      </c>
+      <c r="J16" t="s">
         <v>475</v>
-      </c>
-      <c r="J16" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="17">
@@ -3499,31 +3496,31 @@
         <v>153</v>
       </c>
       <c r="B17" t="s">
+        <v>476</v>
+      </c>
+      <c r="C17" t="s">
         <v>477</v>
       </c>
-      <c r="C17" t="s">
+      <c r="D17" t="s">
         <v>478</v>
       </c>
-      <c r="D17" t="s">
+      <c r="E17" t="s">
         <v>479</v>
       </c>
-      <c r="E17" t="s">
+      <c r="F17" t="s">
         <v>480</v>
       </c>
-      <c r="F17" t="s">
+      <c r="G17" t="s">
         <v>481</v>
-      </c>
-      <c r="G17" t="s">
-        <v>482</v>
       </c>
       <c r="H17" t="s">
         <v>364</v>
       </c>
       <c r="I17" t="s">
+        <v>482</v>
+      </c>
+      <c r="J17" t="s">
         <v>483</v>
-      </c>
-      <c r="J17" t="s">
-        <v>484</v>
       </c>
     </row>
     <row r="18">
@@ -3531,31 +3528,31 @@
         <v>163</v>
       </c>
       <c r="B18" t="s">
+        <v>484</v>
+      </c>
+      <c r="C18" t="s">
         <v>485</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>486</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>487</v>
       </c>
-      <c r="E18" t="s">
+      <c r="F18" t="s">
         <v>488</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>489</v>
-      </c>
-      <c r="G18" t="s">
-        <v>490</v>
       </c>
       <c r="H18" t="s">
         <v>364</v>
       </c>
       <c r="I18" t="s">
+        <v>490</v>
+      </c>
+      <c r="J18" t="s">
         <v>491</v>
-      </c>
-      <c r="J18" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="19">
@@ -3563,60 +3560,60 @@
         <v>173</v>
       </c>
       <c r="B19" t="s">
+        <v>492</v>
+      </c>
+      <c r="C19" t="s">
         <v>493</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>494</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>495</v>
       </c>
-      <c r="E19" t="s">
+      <c r="F19" t="s">
         <v>496</v>
       </c>
-      <c r="F19" t="s">
+      <c r="G19" t="s">
         <v>497</v>
-      </c>
-      <c r="G19" t="s">
-        <v>498</v>
       </c>
       <c r="H19" t="s">
         <v>364</v>
       </c>
       <c r="I19" t="s">
+        <v>498</v>
+      </c>
+      <c r="J19" t="s">
         <v>499</v>
-      </c>
-      <c r="J19" t="s">
-        <v>500</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B20" t="s">
+        <v>500</v>
+      </c>
+      <c r="C20" t="s">
         <v>501</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>502</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>503</v>
       </c>
-      <c r="E20" t="s">
+      <c r="F20" t="s">
         <v>504</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>505</v>
-      </c>
-      <c r="G20" t="s">
-        <v>506</v>
       </c>
       <c r="H20" t="s">
         <v>364</v>
       </c>
       <c r="I20" t="s">
-        <v>501</v>
+        <v>506</v>
       </c>
       <c r="J20" t="s">
         <v>507</v>
@@ -3624,7 +3621,7 @@
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="B21" t="s">
         <v>508</v>
@@ -3648,10 +3645,10 @@
         <v>364</v>
       </c>
       <c r="I21" t="s">
+        <v>508</v>
+      </c>
+      <c r="J21" t="s">
         <v>514</v>
-      </c>
-      <c r="J21" t="s">
-        <v>515</v>
       </c>
     </row>
   </sheetData>

</xml_diff>